<commit_message>
ajout des KPI à school fees
</commit_message>
<xml_diff>
--- a/translations/config.xlsx
+++ b/translations/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="810">
   <si>
     <t>clé</t>
   </si>
@@ -2439,6 +2439,12 @@
   </si>
   <si>
     <t>AAAA</t>
+  </si>
+  <si>
+    <t>display KPI</t>
+  </si>
+  <si>
+    <t>afficher KPI</t>
   </si>
   <si>
     <t>Les prix à l'achat sont promotionnels et sont fonction de la durée choisie</t>
@@ -3666,12 +3672,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C370"/>
+  <dimension ref="A1:C371"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A370" sqref="A370"/>
+      <selection pane="bottomLeft" activeCell="D361" sqref="D361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.5555555555556" defaultRowHeight="15.6" outlineLevelCol="2"/>
@@ -7751,9 +7757,20 @@
         <v>796</v>
       </c>
     </row>
+    <row r="371" spans="1:3">
+      <c r="A371" s="22" t="s">
+        <v>797</v>
+      </c>
+      <c r="B371" s="22" t="s">
+        <v>797</v>
+      </c>
+      <c r="C371" s="22" t="s">
+        <v>798</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:C370" etc:filterBottomFollowUsedRange="0">
-    <sortState ref="A2:C370">
+    <sortState ref="A1:C370">
       <sortCondition ref="A1"/>
     </sortState>
     <extLst/>
@@ -7785,7 +7802,7 @@
   <sheetData>
     <row r="3" spans="2:6">
       <c r="B3" s="6" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -7815,10 +7832,10 @@
     </row>
     <row r="7" ht="27.6" customHeight="1" spans="2:6">
       <c r="B7" s="7" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -7827,27 +7844,27 @@
     <row r="8" s="1" customFormat="1" ht="64.2" customHeight="1" spans="2:8">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>761</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="38.4" customHeight="1" spans="2:11">
       <c r="B9" s="12" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -7875,7 +7892,7 @@
     </row>
     <row r="10" s="2" customFormat="1" ht="38.4" customHeight="1" spans="2:11">
       <c r="B10" s="12" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C10" s="13">
         <f>F10/E10*12</f>
@@ -7922,7 +7939,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="F12" s="9">
         <v>560.5</v>
@@ -8002,10 +8019,10 @@
     </row>
     <row r="7" ht="27.6" customHeight="1" spans="2:6">
       <c r="B7" s="7" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -8014,27 +8031,27 @@
     <row r="8" s="1" customFormat="1" ht="64.2" customHeight="1" spans="2:8">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>761</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="45" customHeight="1" spans="2:11">
       <c r="B9" s="12" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -8062,7 +8079,7 @@
     </row>
     <row r="10" s="2" customFormat="1" ht="38.4" customHeight="1" spans="2:11">
       <c r="B10" s="12" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C10" s="13">
         <f>F10/E10*12</f>
@@ -8109,7 +8126,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="F12" s="9">
         <v>560.5</v>

</xml_diff>